<commit_message>
Sredjen putni nalog i jos neki detalji
</commit_message>
<xml_diff>
--- a/dokumenta/IZ077.xlsx
+++ b/dokumenta/IZ077.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajo\Desktop\IMS\12_IMS_FLOTA\ims_fleet\dokumenta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{086C8B54-DBD4-4EC2-97F3-9C2EA597DE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD00D7CF-3697-42EB-B3C9-2E991A726665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{73934E29-B2A0-4F6A-A874-988B7F2EA183}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{73934E29-B2A0-4F6A-A874-988B7F2EA183}"/>
   </bookViews>
   <sheets>
     <sheet name="zadnja strana" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>ПУТНИ РАЧУН</t>
   </si>
@@ -183,30 +183,16 @@
     <t>Путни трошкови падају на терет / извештај:</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">упућује се на службени пут дана                 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>.2009.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">  У</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">упућује се на службени пут дана     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">упућује се на службени пут дана              </t>
+  </si>
+  <si>
+    <t>у</t>
+  </si>
+  <si>
+    <t xml:space="preserve">у </t>
   </si>
 </sst>
 </file>
@@ -897,12 +883,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -921,16 +906,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -942,13 +927,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -957,7 +941,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
@@ -966,27 +950,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -997,7 +978,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1006,26 +986,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1043,43 +1019,30 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1094,8 +1057,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1114,6 +1077,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1125,58 +1107,75 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1186,23 +1185,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1521,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CCA05F-730E-48AB-BC67-9127058143F9}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25:T25"/>
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1557,555 +1544,556 @@
       <c r="M1" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="P1" s="16"/>
     </row>
     <row r="2" spans="2:20" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="M2" s="4" t="s">
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="M2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="97"/>
-      <c r="O2" s="98"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="83"/>
     </row>
     <row r="3" spans="2:20" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="115"/>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="107"/>
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="111" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="111"/>
-      <c r="J3" s="112" t="s">
+      <c r="I3" s="96"/>
+      <c r="J3" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="113"/>
-      <c r="M3" s="131"/>
-      <c r="N3" s="132"/>
-      <c r="O3" s="132"/>
+      <c r="K3" s="105"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
     </row>
     <row r="4" spans="2:20" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="109"/>
-      <c r="C4" s="107" t="s">
+      <c r="B4" s="94"/>
+      <c r="C4" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="116"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="9"/>
-      <c r="P4" s="128" t="s">
+      <c r="D4" s="108"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+      <c r="P4" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="125"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="125"/>
-    </row>
-    <row r="5" spans="2:20" s="13" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10"/>
-      <c r="C5" s="7" t="s">
+      <c r="Q4" s="116"/>
+      <c r="R4" s="116"/>
+      <c r="S4" s="116"/>
+    </row>
+    <row r="5" spans="2:20" s="12" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="9"/>
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="106" t="s">
+      <c r="E5" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="106"/>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="91"/>
+      <c r="G5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="107" t="s">
+      <c r="H5" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12"/>
-      <c r="N5" s="14"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11"/>
+      <c r="N5" s="13"/>
     </row>
     <row r="6" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="16"/>
-      <c r="M6" s="17" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
+      <c r="M6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="18"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="89"/>
-      <c r="Q6" s="89"/>
-      <c r="R6" s="89"/>
-      <c r="S6" s="89"/>
-      <c r="T6" s="89"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="99"/>
+      <c r="P6" s="100"/>
+      <c r="Q6" s="100"/>
+      <c r="R6" s="100"/>
+      <c r="S6" s="100"/>
+      <c r="T6" s="100"/>
     </row>
     <row r="7" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="110"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="16"/>
-      <c r="M7" s="17" t="s">
+      <c r="B7" s="95"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15"/>
+      <c r="M7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="87"/>
-      <c r="T7" s="87"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="97"/>
+      <c r="S7" s="98"/>
+      <c r="T7" s="98"/>
     </row>
     <row r="8" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="110"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="16"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
-      <c r="P8" s="89"/>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="89"/>
-      <c r="S8" s="89"/>
-      <c r="T8" s="89"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
+      <c r="M8" s="99"/>
+      <c r="N8" s="100"/>
+      <c r="O8" s="100"/>
+      <c r="P8" s="100"/>
+      <c r="Q8" s="100"/>
+      <c r="R8" s="100"/>
+      <c r="S8" s="100"/>
+      <c r="T8" s="100"/>
     </row>
     <row r="9" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="110"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
-      <c r="M9" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="87"/>
-      <c r="T9" s="87"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+      <c r="M9" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="97"/>
+      <c r="S9" s="98"/>
+      <c r="T9" s="98"/>
     </row>
     <row r="10" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="110"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
-      <c r="M10" s="88"/>
-      <c r="N10" s="88"/>
-      <c r="O10" s="88"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="88"/>
-      <c r="S10" s="88"/>
-      <c r="T10" s="22"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
+      <c r="M10" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="99"/>
+      <c r="O10" s="99"/>
+      <c r="P10" s="99"/>
+      <c r="Q10" s="99"/>
+      <c r="R10" s="99"/>
+      <c r="S10" s="99"/>
+      <c r="T10" s="99"/>
     </row>
     <row r="11" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="110"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
-      <c r="M11" s="17" t="s">
+      <c r="B11" s="95"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
+      <c r="M11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="N11" s="18"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="87"/>
-      <c r="Q11" s="87"/>
-      <c r="R11" s="87"/>
-      <c r="S11" s="87"/>
-      <c r="T11" s="87"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="97"/>
+      <c r="P11" s="98"/>
+      <c r="Q11" s="98"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="98"/>
+      <c r="T11" s="98"/>
     </row>
     <row r="12" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="110"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
-      <c r="M12" s="127"/>
-      <c r="N12" s="127"/>
-      <c r="O12" s="127"/>
-      <c r="P12" s="127"/>
-      <c r="Q12" s="127"/>
-      <c r="R12" s="127"/>
-      <c r="S12" s="127"/>
-      <c r="T12" s="127"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15"/>
+      <c r="M12" s="101"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="101"/>
+      <c r="P12" s="101"/>
+      <c r="Q12" s="101"/>
+      <c r="R12" s="101"/>
+      <c r="S12" s="101"/>
+      <c r="T12" s="101"/>
     </row>
     <row r="13" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="110"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="24"/>
-      <c r="M13" s="92"/>
-      <c r="N13" s="92"/>
-      <c r="O13" s="92"/>
-      <c r="P13" s="92"/>
-      <c r="Q13" s="92"/>
-      <c r="R13" s="92"/>
-      <c r="S13" s="92"/>
-      <c r="T13" s="92"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="102"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="102"/>
+      <c r="R13" s="102"/>
+      <c r="S13" s="102"/>
+      <c r="T13" s="102"/>
     </row>
     <row r="14" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="100" t="s">
+      <c r="B14" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="9"/>
-      <c r="M14" s="133"/>
-      <c r="N14" s="93"/>
-      <c r="O14" s="93"/>
-      <c r="P14" s="93"/>
-      <c r="Q14" s="93"/>
-      <c r="R14" s="93"/>
-      <c r="S14" s="93"/>
-      <c r="T14" s="93"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="8"/>
+      <c r="M14" s="121"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="79"/>
+      <c r="R14" s="79"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="79"/>
     </row>
     <row r="15" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="101"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="9"/>
-      <c r="M15" s="17" t="s">
+      <c r="B15" s="86"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="8"/>
+      <c r="M15" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="86"/>
-      <c r="S15" s="86"/>
-      <c r="T15" s="86"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="97"/>
+      <c r="S15" s="97"/>
+      <c r="T15" s="97"/>
     </row>
     <row r="16" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="101"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="9"/>
-      <c r="M16" s="88"/>
-      <c r="N16" s="88"/>
-      <c r="O16" s="88"/>
-      <c r="P16" s="88"/>
-      <c r="Q16" s="88"/>
-      <c r="R16" s="88"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="88"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8"/>
+      <c r="M16" s="99"/>
+      <c r="N16" s="99"/>
+      <c r="O16" s="99"/>
+      <c r="P16" s="99"/>
+      <c r="Q16" s="99"/>
+      <c r="R16" s="99"/>
+      <c r="S16" s="99"/>
+      <c r="T16" s="99"/>
     </row>
     <row r="17" spans="2:20" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31" t="s">
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="32"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="34"/>
-      <c r="M17" s="17" t="s">
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32"/>
+      <c r="M17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="126"/>
-      <c r="T17" s="126"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="125"/>
+      <c r="T17" s="125"/>
     </row>
     <row r="18" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="103" t="s">
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="104"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="104"/>
-      <c r="I18" s="105"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39"/>
-      <c r="M18" s="17" t="s">
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="37"/>
+      <c r="M18" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="88"/>
-      <c r="S18" s="88"/>
-      <c r="T18" s="88"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="99"/>
+      <c r="S18" s="99"/>
+      <c r="T18" s="99"/>
     </row>
     <row r="19" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="29"/>
-      <c r="C19" s="40" t="s">
+      <c r="B19" s="27"/>
+      <c r="C19" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="102" t="s">
+      <c r="D19" s="39"/>
+      <c r="E19" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="102"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="102"/>
-      <c r="I19" s="102"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="9"/>
-      <c r="M19" s="17" t="s">
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="8"/>
+      <c r="M19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="42"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
     </row>
     <row r="20" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="118"/>
-      <c r="H20" s="118"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="118"/>
-      <c r="K20" s="119"/>
-      <c r="M20" s="17" t="s">
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="110"/>
+      <c r="K20" s="111"/>
+      <c r="M20" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="42"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
     </row>
     <row r="21" spans="2:20" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="120" t="s">
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="120"/>
-      <c r="I21" s="120"/>
-      <c r="J21" s="120"/>
-      <c r="K21" s="121"/>
-      <c r="M21" s="17" t="s">
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="113"/>
+      <c r="M21" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
     </row>
     <row r="22" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="M22" s="96" t="s">
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="M22" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="N22" s="96"/>
-      <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="96"/>
+      <c r="N22" s="114"/>
+      <c r="O22" s="114"/>
+      <c r="P22" s="114"/>
+      <c r="Q22" s="114"/>
       <c r="R22" s="122"/>
       <c r="S22" s="123"/>
       <c r="T22" s="123"/>
     </row>
     <row r="23" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="M23" s="96" t="s">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="M23" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="N23" s="125"/>
-      <c r="O23" s="125"/>
-      <c r="P23" s="125"/>
-      <c r="Q23" s="125"/>
-      <c r="R23" s="88"/>
-      <c r="S23" s="88"/>
-      <c r="T23" s="88"/>
+      <c r="N23" s="116"/>
+      <c r="O23" s="116"/>
+      <c r="P23" s="116"/>
+      <c r="Q23" s="116"/>
+      <c r="R23" s="99"/>
+      <c r="S23" s="99"/>
+      <c r="T23" s="99"/>
     </row>
     <row r="24" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="M24" s="127"/>
-      <c r="N24" s="127"/>
-      <c r="O24" s="127"/>
-      <c r="P24" s="127"/>
-      <c r="Q24" s="127"/>
-      <c r="R24" s="127"/>
-      <c r="S24" s="127"/>
-      <c r="T24" s="127"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="M24" s="103"/>
+      <c r="N24" s="103"/>
+      <c r="O24" s="103"/>
+      <c r="P24" s="103"/>
+      <c r="Q24" s="103"/>
+      <c r="R24" s="103"/>
+      <c r="S24" s="103"/>
+      <c r="T24" s="103"/>
     </row>
     <row r="25" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="47"/>
-      <c r="M25" s="92"/>
-      <c r="N25" s="92"/>
-      <c r="O25" s="92"/>
-      <c r="P25" s="92"/>
-      <c r="Q25" s="92"/>
-      <c r="R25" s="92"/>
-      <c r="S25" s="92"/>
-      <c r="T25" s="92"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="78"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="78"/>
     </row>
     <row r="26" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="M26" s="93"/>
-      <c r="N26" s="93"/>
-      <c r="O26" s="93"/>
-      <c r="P26" s="93"/>
-      <c r="Q26" s="93"/>
-      <c r="R26" s="93"/>
-      <c r="S26" s="93"/>
-      <c r="T26" s="93"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="M26" s="79"/>
+      <c r="N26" s="79"/>
+      <c r="O26" s="79"/>
+      <c r="P26" s="79"/>
+      <c r="Q26" s="79"/>
+      <c r="R26" s="79"/>
+      <c r="S26" s="79"/>
+      <c r="T26" s="79"/>
     </row>
     <row r="27" spans="2:20" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F27" s="3"/>
@@ -2113,14 +2101,14 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="M27" s="94"/>
-      <c r="N27" s="94"/>
-      <c r="O27" s="94"/>
-      <c r="P27" s="94"/>
-      <c r="Q27" s="94"/>
-      <c r="R27" s="94"/>
-      <c r="S27" s="94"/>
-      <c r="T27" s="94"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="80"/>
+      <c r="O27" s="80"/>
+      <c r="P27" s="80"/>
+      <c r="Q27" s="80"/>
+      <c r="R27" s="80"/>
+      <c r="S27" s="80"/>
+      <c r="T27" s="80"/>
     </row>
     <row r="28" spans="2:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
@@ -2131,14 +2119,14 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-      <c r="M28" s="95"/>
-      <c r="N28" s="95"/>
-      <c r="O28" s="95"/>
-      <c r="P28" s="95"/>
-      <c r="Q28" s="95"/>
-      <c r="R28" s="95"/>
-      <c r="S28" s="95"/>
-      <c r="T28" s="95"/>
+      <c r="M28" s="81"/>
+      <c r="N28" s="81"/>
+      <c r="O28" s="81"/>
+      <c r="P28" s="81"/>
+      <c r="Q28" s="81"/>
+      <c r="R28" s="81"/>
+      <c r="S28" s="81"/>
+      <c r="T28" s="81"/>
     </row>
     <row r="29" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
@@ -2150,101 +2138,89 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="M29" s="124"/>
-      <c r="N29" s="93"/>
-      <c r="O29" s="93"/>
-      <c r="P29" s="93"/>
-      <c r="Q29" s="93"/>
-      <c r="R29" s="93"/>
-      <c r="S29" s="93"/>
-      <c r="T29" s="93"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="79"/>
+      <c r="P29" s="79"/>
+      <c r="Q29" s="79"/>
+      <c r="R29" s="79"/>
+      <c r="S29" s="79"/>
+      <c r="T29" s="79"/>
     </row>
     <row r="30" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="49"/>
-      <c r="C30" s="50" t="s">
+      <c r="B30" s="45"/>
+      <c r="C30" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="91" t="s">
+      <c r="D30" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="90"/>
+      <c r="E30" s="76"/>
       <c r="F30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G30" s="3"/>
-      <c r="H30" s="91" t="s">
+      <c r="H30" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="I30" s="90"/>
-      <c r="J30" s="117"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="109"/>
     </row>
     <row r="31" spans="2:20" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="49"/>
-      <c r="C31" s="50" t="s">
+      <c r="B31" s="45"/>
+      <c r="C31" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="91"/>
-      <c r="E31" s="90"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="76"/>
       <c r="F31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="91"/>
-      <c r="I31" s="90"/>
-      <c r="J31" s="117"/>
-      <c r="Q31" s="129" t="s">
+      <c r="H31" s="77"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="109"/>
+      <c r="Q31" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="R31" s="130"/>
-      <c r="S31" s="130"/>
+      <c r="R31" s="118"/>
+      <c r="S31" s="118"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C32" s="90" t="s">
+      <c r="C32" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="52"/>
-      <c r="C33" s="53"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="Q33" s="17" t="s">
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="Q33" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="R33" s="37"/>
-      <c r="S33" s="37"/>
-      <c r="T33" s="37"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="35"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="54" t="s">
+      <c r="H34" s="49" t="s">
         <v>19</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
     <row r="35" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="M35" s="14" t="s">
+      <c r="M35" s="13" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="Q31:S31"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="M8:T8"/>
-    <mergeCell ref="M10:S10"/>
-    <mergeCell ref="M12:T12"/>
-    <mergeCell ref="M13:T13"/>
-    <mergeCell ref="M14:T14"/>
-    <mergeCell ref="M16:T16"/>
-    <mergeCell ref="R15:T15"/>
+  <mergeCells count="42">
     <mergeCell ref="R22:T22"/>
     <mergeCell ref="M29:T29"/>
     <mergeCell ref="M23:Q23"/>
@@ -2258,6 +2234,15 @@
     <mergeCell ref="H30:J31"/>
     <mergeCell ref="G20:K20"/>
     <mergeCell ref="G21:K21"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="M22:Q22"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M8:T8"/>
+    <mergeCell ref="M14:T14"/>
+    <mergeCell ref="M16:T16"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B14:B16"/>
@@ -2268,16 +2253,16 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R9:T9"/>
     <mergeCell ref="O11:T11"/>
     <mergeCell ref="O6:T6"/>
+    <mergeCell ref="N10:T10"/>
+    <mergeCell ref="M12:T13"/>
+    <mergeCell ref="R15:T15"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="D30:E31"/>
     <mergeCell ref="M25:T25"/>
     <mergeCell ref="M26:T26"/>
     <mergeCell ref="M27:T28"/>
-    <mergeCell ref="M22:Q22"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.17" right="0.28000000000000003" top="0.21" bottom="0.15" header="0.21" footer="0.15"/>
@@ -2288,10 +2273,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFBF009-0483-4CD7-B9F0-1A1FB65DC806}">
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2309,7 +2294,7 @@
     <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
     <col min="13" max="13" width="5.109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="7.88671875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="1.5546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="1.88671875" style="1" customWidth="1"/>
     <col min="16" max="16" width="5.6640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="22.6640625" style="1" customWidth="1"/>
     <col min="18" max="18" width="9.44140625" style="1" customWidth="1"/>
@@ -2318,630 +2303,623 @@
     <col min="21" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
       <c r="M1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="139" t="s">
+    <row r="2" spans="2:21" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="139"/>
-      <c r="I2" s="139"/>
-      <c r="J2" s="139"/>
-      <c r="K2" s="139"/>
-      <c r="M2" s="4" t="s">
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="137"/>
+      <c r="K2" s="137"/>
+      <c r="M2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="134"/>
-      <c r="O2" s="135"/>
-    </row>
-    <row r="3" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="140"/>
-      <c r="C3" s="147"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="143"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="145"/>
-      <c r="O3" s="146"/>
-    </row>
-    <row r="4" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="140"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="60"/>
-      <c r="P4" s="128" t="s">
+      <c r="N2" s="131"/>
+      <c r="O2" s="132"/>
+    </row>
+    <row r="3" spans="2:21" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="136"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="139"/>
+      <c r="K3" s="140"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="127"/>
+      <c r="O3" s="128"/>
+    </row>
+    <row r="4" spans="2:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="136"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="54"/>
+      <c r="P4" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="137"/>
-      <c r="R4" s="137"/>
-      <c r="S4" s="137"/>
-    </row>
-    <row r="5" spans="2:20" s="13" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="61"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="150"/>
-      <c r="F5" s="150"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="62"/>
-      <c r="N5" s="14"/>
-    </row>
-    <row r="6" spans="2:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="140"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="65"/>
-      <c r="M6" s="17" t="s">
+      <c r="Q4" s="116"/>
+      <c r="R4" s="116"/>
+      <c r="S4" s="116"/>
+    </row>
+    <row r="5" spans="2:21" s="12" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="55"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="56"/>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="136"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="58"/>
+      <c r="M6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="18"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="88"/>
-      <c r="Q6" s="88"/>
-      <c r="R6" s="88"/>
-      <c r="S6" s="88"/>
-      <c r="T6" s="88"/>
-    </row>
-    <row r="7" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="140"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="65"/>
-      <c r="M7" s="17" t="s">
+      <c r="N6" s="17"/>
+      <c r="O6" s="99"/>
+      <c r="P6" s="99"/>
+      <c r="Q6" s="99"/>
+      <c r="R6" s="99"/>
+      <c r="S6" s="99"/>
+      <c r="T6" s="99"/>
+    </row>
+    <row r="7" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="136"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="58"/>
+      <c r="M7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="87"/>
-      <c r="T7" s="87"/>
-    </row>
-    <row r="8" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="140"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="65"/>
-      <c r="M8" s="138"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="88"/>
-      <c r="S8" s="88"/>
-      <c r="T8" s="88"/>
-    </row>
-    <row r="9" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="140"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="65"/>
-      <c r="M9" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="86"/>
-      <c r="T9" s="86"/>
-    </row>
-    <row r="10" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="140"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="65"/>
-      <c r="M10" s="127"/>
-      <c r="N10" s="127"/>
-      <c r="O10" s="127"/>
-      <c r="P10" s="127"/>
-      <c r="Q10" s="127"/>
-      <c r="R10" s="127"/>
-      <c r="S10" s="127"/>
-      <c r="T10" s="127"/>
-    </row>
-    <row r="11" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="140"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="65"/>
-      <c r="M11" s="17" t="s">
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="97"/>
+      <c r="S7" s="98"/>
+      <c r="T7" s="98"/>
+    </row>
+    <row r="8" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="136"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="58"/>
+      <c r="M8" s="134"/>
+      <c r="N8" s="99"/>
+      <c r="O8" s="99"/>
+      <c r="P8" s="99"/>
+      <c r="Q8" s="99"/>
+      <c r="R8" s="99"/>
+      <c r="S8" s="99"/>
+      <c r="T8" s="99"/>
+    </row>
+    <row r="9" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="136"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="58"/>
+      <c r="M9" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="97"/>
+      <c r="S9" s="97"/>
+      <c r="T9" s="97"/>
+    </row>
+    <row r="10" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="136"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="58"/>
+      <c r="M10" s="142" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="143"/>
+      <c r="O10" s="143"/>
+      <c r="P10" s="143"/>
+      <c r="Q10" s="143"/>
+      <c r="R10" s="143"/>
+      <c r="S10" s="143"/>
+      <c r="T10" s="143"/>
+      <c r="U10" s="143"/>
+    </row>
+    <row r="11" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="136"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="58"/>
+      <c r="M11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="N11" s="18"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="87"/>
-      <c r="Q11" s="87"/>
-      <c r="R11" s="87"/>
-      <c r="S11" s="87"/>
-      <c r="T11" s="87"/>
-    </row>
-    <row r="12" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="140"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="65"/>
-      <c r="M12" s="149"/>
-      <c r="N12" s="149"/>
-      <c r="O12" s="149"/>
-      <c r="P12" s="149"/>
-      <c r="Q12" s="149"/>
-      <c r="R12" s="149"/>
-      <c r="S12" s="149"/>
-      <c r="T12" s="149"/>
-    </row>
-    <row r="13" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="140"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="65"/>
-      <c r="M13" s="127"/>
-      <c r="N13" s="127"/>
-      <c r="O13" s="127"/>
-      <c r="P13" s="127"/>
-      <c r="Q13" s="127"/>
-      <c r="R13" s="127"/>
-      <c r="S13" s="127"/>
-      <c r="T13" s="127"/>
-    </row>
-    <row r="14" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="140"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="65"/>
-      <c r="M14" s="136"/>
-      <c r="N14" s="93"/>
-      <c r="O14" s="93"/>
-      <c r="P14" s="93"/>
-      <c r="Q14" s="93"/>
-      <c r="R14" s="93"/>
-      <c r="S14" s="93"/>
-      <c r="T14" s="93"/>
-    </row>
-    <row r="15" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="140"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="65"/>
-      <c r="M15" s="17" t="s">
+      <c r="N11" s="17"/>
+      <c r="O11" s="97"/>
+      <c r="P11" s="98"/>
+      <c r="Q11" s="98"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="98"/>
+      <c r="T11" s="98"/>
+    </row>
+    <row r="12" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="136"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="58"/>
+      <c r="M12" s="141"/>
+      <c r="N12" s="141"/>
+      <c r="O12" s="141"/>
+      <c r="P12" s="141"/>
+      <c r="Q12" s="141"/>
+      <c r="R12" s="141"/>
+      <c r="S12" s="141"/>
+      <c r="T12" s="141"/>
+    </row>
+    <row r="13" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="136"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="58"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="103"/>
+      <c r="O13" s="103"/>
+      <c r="P13" s="103"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="103"/>
+      <c r="S13" s="103"/>
+      <c r="T13" s="103"/>
+    </row>
+    <row r="14" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="136"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="58"/>
+      <c r="M14" s="133"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="79"/>
+      <c r="R14" s="79"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="79"/>
+    </row>
+    <row r="15" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="136"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="58"/>
+      <c r="M15" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="86"/>
-      <c r="S15" s="86"/>
-      <c r="T15" s="86"/>
-    </row>
-    <row r="16" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="140"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="65"/>
-      <c r="M16" s="88"/>
-      <c r="N16" s="88"/>
-      <c r="O16" s="88"/>
-      <c r="P16" s="88"/>
-      <c r="Q16" s="88"/>
-      <c r="R16" s="88"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="88"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="97"/>
+      <c r="S15" s="97"/>
+      <c r="T15" s="97"/>
+    </row>
+    <row r="16" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="136"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="58"/>
+      <c r="M16" s="99"/>
+      <c r="N16" s="99"/>
+      <c r="O16" s="99"/>
+      <c r="P16" s="99"/>
+      <c r="Q16" s="99"/>
+      <c r="R16" s="99"/>
+      <c r="S16" s="99"/>
+      <c r="T16" s="99"/>
     </row>
     <row r="17" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="63"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="65"/>
-      <c r="M17" s="17" t="s">
+      <c r="C17" s="57"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="58"/>
+      <c r="M17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="126"/>
-      <c r="T17" s="126"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="125"/>
+      <c r="T17" s="125"/>
     </row>
     <row r="18" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="63"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="93"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="65"/>
-      <c r="M18" s="17" t="s">
+      <c r="C18" s="57"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="58"/>
+      <c r="M18" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="88"/>
-      <c r="S18" s="88"/>
-      <c r="T18" s="88"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="99"/>
+      <c r="S18" s="99"/>
+      <c r="T18" s="99"/>
     </row>
     <row r="19" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="63"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="65"/>
-      <c r="M19" s="17" t="s">
+      <c r="C19" s="57"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="98"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="58"/>
+      <c r="M19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="42"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
     </row>
     <row r="20" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="63"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="67"/>
-      <c r="M20" s="17" t="s">
+      <c r="C20" s="57"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="58"/>
+      <c r="M20" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="42"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
     </row>
     <row r="21" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="63"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="68"/>
-      <c r="M21" s="17" t="s">
+      <c r="C21" s="57"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="60"/>
+      <c r="M21" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
     </row>
     <row r="22" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="63"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="68"/>
-      <c r="M22" s="17" t="s">
+      <c r="C22" s="57"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="60"/>
+      <c r="M22" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
       <c r="R22" s="122"/>
       <c r="S22" s="123"/>
       <c r="T22" s="123"/>
     </row>
     <row r="23" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="69"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="67"/>
-      <c r="M23" s="96" t="s">
+      <c r="C23" s="61"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="58"/>
+      <c r="M23" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="N23" s="125"/>
-      <c r="O23" s="125"/>
-      <c r="P23" s="125"/>
-      <c r="Q23" s="125"/>
-      <c r="R23" s="88"/>
-      <c r="S23" s="88"/>
-      <c r="T23" s="88"/>
+      <c r="N23" s="116"/>
+      <c r="O23" s="116"/>
+      <c r="P23" s="116"/>
+      <c r="Q23" s="116"/>
+      <c r="R23" s="99"/>
+      <c r="S23" s="99"/>
+      <c r="T23" s="99"/>
     </row>
     <row r="24" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="67"/>
-      <c r="M24" s="95"/>
-      <c r="N24" s="95"/>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="95"/>
-      <c r="S24" s="95"/>
-      <c r="T24" s="95"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="58"/>
+      <c r="M24" s="81"/>
+      <c r="N24" s="81"/>
+      <c r="O24" s="81"/>
+      <c r="P24" s="81"/>
+      <c r="Q24" s="81"/>
+      <c r="R24" s="81"/>
+      <c r="S24" s="81"/>
+      <c r="T24" s="81"/>
     </row>
     <row r="25" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="42"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="67"/>
-      <c r="M25" s="93"/>
-      <c r="N25" s="93"/>
-      <c r="O25" s="93"/>
-      <c r="P25" s="93"/>
-      <c r="Q25" s="93"/>
-      <c r="R25" s="93"/>
-      <c r="S25" s="93"/>
-      <c r="T25" s="93"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="58"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="79"/>
+      <c r="P25" s="79"/>
+      <c r="Q25" s="79"/>
+      <c r="R25" s="79"/>
+      <c r="S25" s="79"/>
+      <c r="T25" s="79"/>
     </row>
     <row r="26" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="69"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="67"/>
-      <c r="M26" s="93"/>
-      <c r="N26" s="93"/>
-      <c r="O26" s="93"/>
-      <c r="P26" s="93"/>
-      <c r="Q26" s="93"/>
-      <c r="R26" s="93"/>
-      <c r="S26" s="93"/>
-      <c r="T26" s="93"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="58"/>
+      <c r="M26" s="79"/>
+      <c r="N26" s="79"/>
+      <c r="O26" s="79"/>
+      <c r="P26" s="79"/>
+      <c r="Q26" s="79"/>
+      <c r="R26" s="79"/>
+      <c r="S26" s="79"/>
+      <c r="T26" s="79"/>
     </row>
     <row r="27" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="69"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="67"/>
-      <c r="M27" s="93"/>
-      <c r="N27" s="93"/>
-      <c r="O27" s="93"/>
-      <c r="P27" s="93"/>
-      <c r="Q27" s="93"/>
-      <c r="R27" s="93"/>
-      <c r="S27" s="93"/>
-      <c r="T27" s="93"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="58"/>
+      <c r="M27" s="79"/>
+      <c r="N27" s="79"/>
+      <c r="O27" s="79"/>
+      <c r="P27" s="79"/>
+      <c r="Q27" s="79"/>
+      <c r="R27" s="79"/>
+      <c r="S27" s="79"/>
+      <c r="T27" s="79"/>
     </row>
     <row r="28" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="63"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="68"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="60"/>
       <c r="M28" s="124"/>
-      <c r="N28" s="93"/>
-      <c r="O28" s="93"/>
-      <c r="P28" s="93"/>
-      <c r="Q28" s="93"/>
-      <c r="R28" s="93"/>
-      <c r="S28" s="93"/>
-      <c r="T28" s="93"/>
+      <c r="N28" s="79"/>
+      <c r="O28" s="79"/>
+      <c r="P28" s="79"/>
+      <c r="Q28" s="79"/>
+      <c r="R28" s="79"/>
+      <c r="S28" s="79"/>
+      <c r="T28" s="79"/>
     </row>
     <row r="29" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="63"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="65"/>
-      <c r="R29" s="73"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="58"/>
     </row>
     <row r="30" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="63"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="65"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="74"/>
-      <c r="S30" s="75" t="s">
+      <c r="C30" s="57"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="58"/>
+      <c r="Q30" s="47"/>
+      <c r="R30" s="64"/>
+      <c r="S30" s="65" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="31" spans="2:20" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="76"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="60"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="54"/>
     </row>
     <row r="32" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="79"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="82"/>
-      <c r="G32" s="82"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="81"/>
-      <c r="J32" s="83"/>
-      <c r="K32" s="84"/>
-      <c r="Q32" s="85" t="s">
+      <c r="C32" s="69"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="73"/>
+      <c r="Q32" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="R32" s="37"/>
-      <c r="S32" s="37"/>
-      <c r="T32" s="37"/>
+      <c r="R32" s="35"/>
+      <c r="S32" s="35"/>
+      <c r="T32" s="35"/>
     </row>
     <row r="33" spans="3:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M33" s="14" t="s">
+      <c r="M33" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="R33" s="30"/>
-      <c r="S33" s="30"/>
-      <c r="T33" s="30"/>
+      <c r="R33" s="28"/>
+      <c r="S33" s="28"/>
+      <c r="T33" s="28"/>
     </row>
     <row r="34" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="42"/>
-    </row>
-    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="35">
@@ -2951,6 +2929,8 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="E19:I19"/>
     <mergeCell ref="E18:I18"/>
+    <mergeCell ref="M12:T12"/>
+    <mergeCell ref="N10:U10"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="B6:B13"/>
@@ -2971,7 +2951,6 @@
     <mergeCell ref="P4:S4"/>
     <mergeCell ref="M8:T8"/>
     <mergeCell ref="O11:T11"/>
-    <mergeCell ref="M10:T10"/>
     <mergeCell ref="M27:T27"/>
     <mergeCell ref="R22:T22"/>
     <mergeCell ref="M23:Q23"/>
@@ -2979,7 +2958,6 @@
     <mergeCell ref="M24:T24"/>
     <mergeCell ref="M25:T25"/>
     <mergeCell ref="M26:T26"/>
-    <mergeCell ref="M12:T12"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0" right="0.28000000000000003" top="0.22" bottom="0.196850393700787" header="0.28000000000000003" footer="0.196850393700787"/>

</xml_diff>

<commit_message>
Lista dugovanja po baketima
</commit_message>
<xml_diff>
--- a/dokumenta/IZ077.xlsx
+++ b/dokumenta/IZ077.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajo\Desktop\IMS\12_IMS_FLOTA\ims_fleet\dokumenta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD00D7CF-3697-42EB-B3C9-2E991A726665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C032BE4F-E736-4A09-B880-EFBC35B742B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{73934E29-B2A0-4F6A-A874-988B7F2EA183}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{73934E29-B2A0-4F6A-A874-988B7F2EA183}"/>
   </bookViews>
   <sheets>
     <sheet name="zadnja strana" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>ПУТНИ РАЧУН</t>
   </si>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t xml:space="preserve">у </t>
+  </si>
+  <si>
+    <t>дана</t>
+  </si>
+  <si>
+    <t>43/25-23</t>
+  </si>
+  <si>
+    <t>Број:</t>
   </si>
 </sst>
 </file>
@@ -883,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1026,74 +1035,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1106,7 +1061,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1116,11 +1080,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1133,16 +1099,77 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1157,39 +1184,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1508,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CCA05F-730E-48AB-BC67-9127058143F9}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22:T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1547,32 +1553,32 @@
       <c r="P1" s="16"/>
     </row>
     <row r="2" spans="2:20" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
       <c r="M2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="82"/>
-      <c r="O2" s="83"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="107"/>
     </row>
     <row r="3" spans="2:20" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="106" t="s">
+      <c r="C3" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="107"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1580,24 +1586,24 @@
         <v>5</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="96" t="s">
+      <c r="H3" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="96"/>
-      <c r="J3" s="104" t="s">
+      <c r="I3" s="119"/>
+      <c r="J3" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="105"/>
-      <c r="M3" s="119"/>
-      <c r="N3" s="120"/>
-      <c r="O3" s="120"/>
+      <c r="K3" s="85"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
     </row>
     <row r="4" spans="2:20" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="94"/>
-      <c r="C4" s="92" t="s">
+      <c r="B4" s="117"/>
+      <c r="C4" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="108"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1605,12 +1611,12 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="8"/>
-      <c r="P4" s="115" t="s">
+      <c r="P4" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="116"/>
-      <c r="R4" s="116"/>
-      <c r="S4" s="116"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
     </row>
     <row r="5" spans="2:20" s="12" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
@@ -1620,23 +1626,23 @@
       <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="91" t="s">
+      <c r="E5" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="91"/>
+      <c r="F5" s="115"/>
       <c r="G5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="92" t="s">
+      <c r="H5" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="92"/>
+      <c r="I5" s="88"/>
       <c r="J5" s="10"/>
       <c r="K5" s="11"/>
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="118" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="7"/>
@@ -1652,15 +1658,15 @@
         <v>28</v>
       </c>
       <c r="N6" s="17"/>
-      <c r="O6" s="99"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="100"/>
-      <c r="R6" s="100"/>
-      <c r="S6" s="100"/>
-      <c r="T6" s="100"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="104"/>
+      <c r="Q6" s="104"/>
+      <c r="R6" s="104"/>
+      <c r="S6" s="104"/>
+      <c r="T6" s="104"/>
     </row>
     <row r="7" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="95"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1682,7 +1688,7 @@
       <c r="T7" s="98"/>
     </row>
     <row r="8" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="95"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1692,17 +1698,17 @@
       <c r="I8" s="7"/>
       <c r="J8" s="14"/>
       <c r="K8" s="15"/>
-      <c r="M8" s="99"/>
-      <c r="N8" s="100"/>
-      <c r="O8" s="100"/>
-      <c r="P8" s="100"/>
-      <c r="Q8" s="100"/>
-      <c r="R8" s="100"/>
-      <c r="S8" s="100"/>
-      <c r="T8" s="100"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="104"/>
+      <c r="O8" s="104"/>
+      <c r="P8" s="104"/>
+      <c r="Q8" s="104"/>
+      <c r="R8" s="104"/>
+      <c r="S8" s="104"/>
+      <c r="T8" s="104"/>
     </row>
     <row r="9" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1724,7 +1730,7 @@
       <c r="T9" s="98"/>
     </row>
     <row r="10" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="95"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1737,16 +1743,16 @@
       <c r="M10" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="N10" s="99"/>
-      <c r="O10" s="99"/>
-      <c r="P10" s="99"/>
-      <c r="Q10" s="99"/>
-      <c r="R10" s="99"/>
-      <c r="S10" s="99"/>
-      <c r="T10" s="99"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="82"/>
+      <c r="S10" s="82"/>
+      <c r="T10" s="82"/>
     </row>
     <row r="11" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="95"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1768,7 +1774,7 @@
       <c r="T11" s="98"/>
     </row>
     <row r="12" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="95"/>
+      <c r="B12" s="118"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1778,17 +1784,17 @@
       <c r="I12" s="7"/>
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
-      <c r="M12" s="101"/>
-      <c r="N12" s="101"/>
-      <c r="O12" s="101"/>
-      <c r="P12" s="101"/>
-      <c r="Q12" s="101"/>
-      <c r="R12" s="101"/>
-      <c r="S12" s="101"/>
-      <c r="T12" s="101"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
+      <c r="O12" s="120"/>
+      <c r="P12" s="120"/>
+      <c r="Q12" s="120"/>
+      <c r="R12" s="120"/>
+      <c r="S12" s="120"/>
+      <c r="T12" s="120"/>
     </row>
     <row r="13" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="95"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1798,17 +1804,17 @@
       <c r="I13" s="7"/>
       <c r="J13" s="21"/>
       <c r="K13" s="22"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="102"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="102"/>
-      <c r="R13" s="102"/>
-      <c r="S13" s="102"/>
-      <c r="T13" s="102"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="121"/>
+      <c r="O13" s="121"/>
+      <c r="P13" s="121"/>
+      <c r="Q13" s="121"/>
+      <c r="R13" s="121"/>
+      <c r="S13" s="121"/>
+      <c r="T13" s="121"/>
     </row>
     <row r="14" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="109" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="23"/>
@@ -1820,17 +1826,17 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="8"/>
-      <c r="M14" s="121"/>
-      <c r="N14" s="79"/>
-      <c r="O14" s="79"/>
-      <c r="P14" s="79"/>
-      <c r="Q14" s="79"/>
-      <c r="R14" s="79"/>
-      <c r="S14" s="79"/>
-      <c r="T14" s="79"/>
+      <c r="M14" s="105"/>
+      <c r="N14" s="78"/>
+      <c r="O14" s="78"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
+      <c r="S14" s="78"/>
+      <c r="T14" s="78"/>
     </row>
     <row r="15" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="86"/>
+      <c r="B15" s="110"/>
       <c r="C15" s="23"/>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
@@ -1852,7 +1858,7 @@
       <c r="T15" s="97"/>
     </row>
     <row r="16" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="86"/>
+      <c r="B16" s="110"/>
       <c r="C16" s="23"/>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
@@ -1862,14 +1868,14 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="8"/>
-      <c r="M16" s="99"/>
-      <c r="N16" s="99"/>
-      <c r="O16" s="99"/>
-      <c r="P16" s="99"/>
-      <c r="Q16" s="99"/>
-      <c r="R16" s="99"/>
-      <c r="S16" s="99"/>
-      <c r="T16" s="99"/>
+      <c r="M16" s="82"/>
+      <c r="N16" s="82"/>
+      <c r="O16" s="82"/>
+      <c r="P16" s="82"/>
+      <c r="Q16" s="82"/>
+      <c r="R16" s="82"/>
+      <c r="S16" s="82"/>
+      <c r="T16" s="82"/>
     </row>
     <row r="17" spans="2:20" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="27"/>
@@ -1892,20 +1898,20 @@
       <c r="P17" s="33"/>
       <c r="Q17" s="33"/>
       <c r="R17" s="33"/>
-      <c r="S17" s="125"/>
-      <c r="T17" s="125"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
     </row>
     <row r="18" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="34"/>
       <c r="C18" s="35"/>
       <c r="D18" s="35"/>
-      <c r="E18" s="88" t="s">
+      <c r="E18" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="89"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="89"/>
-      <c r="I18" s="90"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="113"/>
+      <c r="I18" s="114"/>
       <c r="J18" s="36"/>
       <c r="K18" s="37"/>
       <c r="M18" s="16" t="s">
@@ -1915,9 +1921,11 @@
       <c r="O18" s="33"/>
       <c r="P18" s="33"/>
       <c r="Q18" s="33"/>
-      <c r="R18" s="99"/>
-      <c r="S18" s="99"/>
-      <c r="T18" s="99"/>
+      <c r="R18" s="82"/>
+      <c r="S18" s="82"/>
+      <c r="T18" s="139" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="27"/>
@@ -1925,13 +1933,13 @@
         <v>17</v>
       </c>
       <c r="D19" s="39"/>
-      <c r="E19" s="87" t="s">
+      <c r="E19" s="111" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="111"/>
       <c r="J19" s="7"/>
       <c r="K19" s="8"/>
       <c r="M19" s="16" t="s">
@@ -1950,11 +1958,11 @@
       </c>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="110"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="111"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="94"/>
       <c r="M20" s="16" t="s">
         <v>47</v>
       </c>
@@ -1971,13 +1979,13 @@
       <c r="D21" s="42"/>
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
-      <c r="G21" s="112" t="s">
+      <c r="G21" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="112"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="112"/>
-      <c r="K21" s="113"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="95"/>
+      <c r="K21" s="96"/>
       <c r="M21" s="16" t="s">
         <v>48</v>
       </c>
@@ -1994,16 +2002,16 @@
       <c r="I22" s="43"/>
       <c r="J22" s="43"/>
       <c r="K22" s="43"/>
-      <c r="M22" s="114" t="s">
+      <c r="M22" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="N22" s="114"/>
-      <c r="O22" s="114"/>
-      <c r="P22" s="114"/>
-      <c r="Q22" s="114"/>
-      <c r="R22" s="122"/>
-      <c r="S22" s="123"/>
-      <c r="T22" s="123"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="79"/>
+      <c r="Q22" s="79"/>
+      <c r="R22" s="142"/>
+      <c r="S22" s="142"/>
+      <c r="T22" s="142"/>
     </row>
     <row r="23" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
@@ -2018,16 +2026,16 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="M23" s="114" t="s">
+      <c r="M23" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="N23" s="116"/>
-      <c r="O23" s="116"/>
-      <c r="P23" s="116"/>
-      <c r="Q23" s="116"/>
-      <c r="R23" s="99"/>
-      <c r="S23" s="99"/>
-      <c r="T23" s="99"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="82"/>
+      <c r="S23" s="82"/>
+      <c r="T23" s="82"/>
     </row>
     <row r="24" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
@@ -2042,14 +2050,14 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="M24" s="103"/>
-      <c r="N24" s="103"/>
-      <c r="O24" s="103"/>
-      <c r="P24" s="103"/>
-      <c r="Q24" s="103"/>
-      <c r="R24" s="103"/>
-      <c r="S24" s="103"/>
-      <c r="T24" s="103"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="83"/>
+      <c r="O24" s="83"/>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="83"/>
+      <c r="R24" s="83"/>
+      <c r="S24" s="83"/>
+      <c r="T24" s="83"/>
     </row>
     <row r="25" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
@@ -2064,14 +2072,14 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-      <c r="M25" s="78"/>
-      <c r="N25" s="78"/>
-      <c r="O25" s="78"/>
-      <c r="P25" s="78"/>
-      <c r="Q25" s="78"/>
-      <c r="R25" s="78"/>
-      <c r="S25" s="78"/>
-      <c r="T25" s="78"/>
+      <c r="M25" s="122"/>
+      <c r="N25" s="122"/>
+      <c r="O25" s="122"/>
+      <c r="P25" s="122"/>
+      <c r="Q25" s="122"/>
+      <c r="R25" s="122"/>
+      <c r="S25" s="122"/>
+      <c r="T25" s="122"/>
     </row>
     <row r="26" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
@@ -2086,14 +2094,14 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="M26" s="79"/>
-      <c r="N26" s="79"/>
-      <c r="O26" s="79"/>
-      <c r="P26" s="79"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="79"/>
-      <c r="S26" s="79"/>
-      <c r="T26" s="79"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="78"/>
+      <c r="O26" s="78"/>
+      <c r="P26" s="78"/>
+      <c r="Q26" s="78"/>
+      <c r="R26" s="78"/>
+      <c r="S26" s="78"/>
+      <c r="T26" s="78"/>
     </row>
     <row r="27" spans="2:20" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F27" s="3"/>
@@ -2101,14 +2109,14 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="M27" s="80"/>
-      <c r="N27" s="80"/>
-      <c r="O27" s="80"/>
-      <c r="P27" s="80"/>
-      <c r="Q27" s="80"/>
-      <c r="R27" s="80"/>
-      <c r="S27" s="80"/>
-      <c r="T27" s="80"/>
+      <c r="M27" s="123"/>
+      <c r="N27" s="123"/>
+      <c r="O27" s="123"/>
+      <c r="P27" s="123"/>
+      <c r="Q27" s="123"/>
+      <c r="R27" s="123"/>
+      <c r="S27" s="123"/>
+      <c r="T27" s="123"/>
     </row>
     <row r="28" spans="2:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
@@ -2119,14 +2127,14 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-      <c r="M28" s="81"/>
-      <c r="N28" s="81"/>
-      <c r="O28" s="81"/>
-      <c r="P28" s="81"/>
-      <c r="Q28" s="81"/>
-      <c r="R28" s="81"/>
-      <c r="S28" s="81"/>
-      <c r="T28" s="81"/>
+      <c r="M28" s="124"/>
+      <c r="N28" s="124"/>
+      <c r="O28" s="124"/>
+      <c r="P28" s="124"/>
+      <c r="Q28" s="124"/>
+      <c r="R28" s="124"/>
+      <c r="S28" s="124"/>
+      <c r="T28" s="124"/>
     </row>
     <row r="29" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
@@ -2137,60 +2145,60 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
-      <c r="M29" s="124"/>
-      <c r="N29" s="79"/>
-      <c r="O29" s="79"/>
-      <c r="P29" s="79"/>
-      <c r="Q29" s="79"/>
-      <c r="R29" s="79"/>
-      <c r="S29" s="79"/>
-      <c r="T29" s="79"/>
+      <c r="M29" s="77"/>
+      <c r="N29" s="78"/>
+      <c r="O29" s="78"/>
+      <c r="P29" s="78"/>
+      <c r="Q29" s="78"/>
+      <c r="R29" s="78"/>
+      <c r="S29" s="78"/>
+      <c r="T29" s="78"/>
     </row>
     <row r="30" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="45"/>
       <c r="C30" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="77" t="s">
+      <c r="D30" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="76"/>
+      <c r="E30" s="91"/>
       <c r="F30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G30" s="3"/>
-      <c r="H30" s="77" t="s">
+      <c r="H30" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="I30" s="76"/>
-      <c r="J30" s="109"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="92"/>
     </row>
     <row r="31" spans="2:20" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="45"/>
       <c r="C31" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="77"/>
-      <c r="E31" s="76"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="91"/>
       <c r="F31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="76"/>
-      <c r="J31" s="109"/>
-      <c r="Q31" s="117" t="s">
+      <c r="H31" s="90"/>
+      <c r="I31" s="91"/>
+      <c r="J31" s="92"/>
+      <c r="Q31" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="R31" s="118"/>
-      <c r="S31" s="118"/>
+      <c r="R31" s="101"/>
+      <c r="S31" s="101"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C32" s="76" t="s">
+      <c r="C32" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="91"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="48"/>
@@ -2221,29 +2229,11 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="M29:T29"/>
-    <mergeCell ref="M23:Q23"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="M24:T24"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="H30:J31"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="G21:K21"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="M22:Q22"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="Q31:S31"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="M8:T8"/>
-    <mergeCell ref="M14:T14"/>
-    <mergeCell ref="M16:T16"/>
-    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="M25:T25"/>
+    <mergeCell ref="M26:T26"/>
+    <mergeCell ref="M27:T28"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="E19:I19"/>
@@ -2253,16 +2243,34 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M8:T8"/>
+    <mergeCell ref="M14:T14"/>
+    <mergeCell ref="M16:T16"/>
+    <mergeCell ref="N2:O2"/>
     <mergeCell ref="O11:T11"/>
     <mergeCell ref="O6:T6"/>
     <mergeCell ref="N10:T10"/>
     <mergeCell ref="M12:T13"/>
     <mergeCell ref="R15:T15"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="D30:E31"/>
-    <mergeCell ref="M25:T25"/>
-    <mergeCell ref="M26:T26"/>
-    <mergeCell ref="M27:T28"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="M22:Q22"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H30:J31"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="M29:T29"/>
+    <mergeCell ref="M23:Q23"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="M24:T24"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.17" right="0.28000000000000003" top="0.21" bottom="0.15" header="0.21" footer="0.15"/>
@@ -2276,7 +2284,7 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13:T13"/>
+      <selection activeCell="O6" sqref="O6:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2293,8 +2301,8 @@
     <col min="11" max="11" width="17.5546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
     <col min="13" max="13" width="5.109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.88671875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="1.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.21875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="3" style="1" customWidth="1"/>
     <col min="16" max="16" width="5.6640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="22.6640625" style="1" customWidth="1"/>
     <col min="18" max="18" width="9.44140625" style="1" customWidth="1"/>
@@ -2318,41 +2326,44 @@
       </c>
     </row>
     <row r="2" spans="2:21" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
       <c r="M2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="131"/>
-      <c r="O2" s="132"/>
+        <v>59</v>
+      </c>
+      <c r="N2" s="140" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="140"/>
+      <c r="P2" s="140"/>
     </row>
     <row r="3" spans="2:21" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="136"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="130"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="136"/>
       <c r="E3" s="50"/>
       <c r="F3" s="50"/>
       <c r="G3" s="51"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="138"/>
-      <c r="J3" s="139"/>
-      <c r="K3" s="140"/>
-      <c r="M3" s="126"/>
-      <c r="N3" s="127"/>
-      <c r="O3" s="128"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="131"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="133"/>
+      <c r="O3" s="134"/>
     </row>
     <row r="4" spans="2:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="136"/>
+      <c r="B4" s="125"/>
       <c r="C4" s="52"/>
       <c r="D4" s="53"/>
       <c r="E4" s="44"/>
@@ -2362,27 +2373,27 @@
       <c r="I4" s="44"/>
       <c r="J4" s="44"/>
       <c r="K4" s="54"/>
-      <c r="P4" s="115" t="s">
+      <c r="P4" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="116"/>
-      <c r="R4" s="116"/>
-      <c r="S4" s="116"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
     </row>
     <row r="5" spans="2:21" s="12" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="55"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="135"/>
-      <c r="F5" s="135"/>
+      <c r="E5" s="127"/>
+      <c r="F5" s="127"/>
       <c r="G5" s="18"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
       <c r="J5" s="18"/>
       <c r="K5" s="56"/>
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="136"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="57"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -2396,15 +2407,15 @@
         <v>28</v>
       </c>
       <c r="N6" s="17"/>
-      <c r="O6" s="99"/>
-      <c r="P6" s="99"/>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="99"/>
-      <c r="S6" s="99"/>
-      <c r="T6" s="99"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
     </row>
     <row r="7" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="136"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="57"/>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -2426,7 +2437,7 @@
       <c r="T7" s="98"/>
     </row>
     <row r="8" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="136"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="57"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
@@ -2436,17 +2447,17 @@
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
       <c r="K8" s="58"/>
-      <c r="M8" s="134"/>
-      <c r="N8" s="99"/>
-      <c r="O8" s="99"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="99"/>
-      <c r="R8" s="99"/>
-      <c r="S8" s="99"/>
-      <c r="T8" s="99"/>
+      <c r="M8" s="138"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="82"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="82"/>
+      <c r="S8" s="82"/>
+      <c r="T8" s="82"/>
     </row>
     <row r="9" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="136"/>
+      <c r="B9" s="125"/>
       <c r="C9" s="57"/>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
@@ -2468,7 +2479,7 @@
       <c r="T9" s="97"/>
     </row>
     <row r="10" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="136"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="57"/>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -2478,20 +2489,20 @@
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
       <c r="K10" s="58"/>
-      <c r="M10" s="142" t="s">
+      <c r="M10" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="143"/>
-      <c r="O10" s="143"/>
-      <c r="P10" s="143"/>
-      <c r="Q10" s="143"/>
-      <c r="R10" s="143"/>
-      <c r="S10" s="143"/>
-      <c r="T10" s="143"/>
-      <c r="U10" s="143"/>
+      <c r="N10" s="126"/>
+      <c r="O10" s="126"/>
+      <c r="P10" s="126"/>
+      <c r="Q10" s="126"/>
+      <c r="R10" s="126"/>
+      <c r="S10" s="126"/>
+      <c r="T10" s="126"/>
+      <c r="U10" s="126"/>
     </row>
     <row r="11" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="136"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="57"/>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
@@ -2513,7 +2524,7 @@
       <c r="T11" s="98"/>
     </row>
     <row r="12" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="136"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="57"/>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
@@ -2533,7 +2544,7 @@
       <c r="T12" s="141"/>
     </row>
     <row r="13" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="136"/>
+      <c r="B13" s="125"/>
       <c r="C13" s="57"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
@@ -2543,17 +2554,17 @@
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
       <c r="K13" s="58"/>
-      <c r="M13" s="103"/>
-      <c r="N13" s="103"/>
-      <c r="O13" s="103"/>
-      <c r="P13" s="103"/>
-      <c r="Q13" s="103"/>
-      <c r="R13" s="103"/>
-      <c r="S13" s="103"/>
-      <c r="T13" s="103"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="82"/>
+      <c r="R13" s="82"/>
+      <c r="S13" s="82"/>
+      <c r="T13" s="82"/>
     </row>
     <row r="14" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="136"/>
+      <c r="B14" s="125"/>
       <c r="C14" s="57"/>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
@@ -2563,17 +2574,17 @@
       <c r="I14" s="26"/>
       <c r="J14" s="26"/>
       <c r="K14" s="58"/>
-      <c r="M14" s="133"/>
-      <c r="N14" s="79"/>
-      <c r="O14" s="79"/>
-      <c r="P14" s="79"/>
-      <c r="Q14" s="79"/>
-      <c r="R14" s="79"/>
-      <c r="S14" s="79"/>
-      <c r="T14" s="79"/>
+      <c r="M14" s="137"/>
+      <c r="N14" s="78"/>
+      <c r="O14" s="78"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
+      <c r="S14" s="78"/>
+      <c r="T14" s="78"/>
     </row>
     <row r="15" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="136"/>
+      <c r="B15" s="125"/>
       <c r="C15" s="57"/>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
@@ -2595,7 +2606,7 @@
       <c r="T15" s="97"/>
     </row>
     <row r="16" spans="2:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="136"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="57"/>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
@@ -2605,14 +2616,14 @@
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="58"/>
-      <c r="M16" s="99"/>
-      <c r="N16" s="99"/>
-      <c r="O16" s="99"/>
-      <c r="P16" s="99"/>
-      <c r="Q16" s="99"/>
-      <c r="R16" s="99"/>
-      <c r="S16" s="99"/>
-      <c r="T16" s="99"/>
+      <c r="M16" s="82"/>
+      <c r="N16" s="82"/>
+      <c r="O16" s="82"/>
+      <c r="P16" s="82"/>
+      <c r="Q16" s="82"/>
+      <c r="R16" s="82"/>
+      <c r="S16" s="82"/>
+      <c r="T16" s="82"/>
     </row>
     <row r="17" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="57"/>
@@ -2632,17 +2643,17 @@
       <c r="P17" s="33"/>
       <c r="Q17" s="33"/>
       <c r="R17" s="33"/>
-      <c r="S17" s="125"/>
-      <c r="T17" s="125"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
     </row>
     <row r="18" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="57"/>
       <c r="D18" s="26"/>
       <c r="E18" s="98"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
       <c r="J18" s="26"/>
       <c r="K18" s="58"/>
       <c r="M18" s="16" t="s">
@@ -2652,9 +2663,11 @@
       <c r="O18" s="33"/>
       <c r="P18" s="33"/>
       <c r="Q18" s="33"/>
-      <c r="R18" s="99"/>
-      <c r="S18" s="99"/>
-      <c r="T18" s="99"/>
+      <c r="R18" s="82"/>
+      <c r="S18" s="82"/>
+      <c r="T18" s="139" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="57"/>
@@ -2733,9 +2746,9 @@
       <c r="O22" s="16"/>
       <c r="P22" s="16"/>
       <c r="Q22" s="16"/>
-      <c r="R22" s="122"/>
-      <c r="S22" s="123"/>
-      <c r="T22" s="123"/>
+      <c r="R22" s="142"/>
+      <c r="S22" s="142"/>
+      <c r="T22" s="142"/>
     </row>
     <row r="23" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="61"/>
@@ -2747,16 +2760,16 @@
       <c r="I23" s="26"/>
       <c r="J23" s="26"/>
       <c r="K23" s="58"/>
-      <c r="M23" s="114" t="s">
+      <c r="M23" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="N23" s="116"/>
-      <c r="O23" s="116"/>
-      <c r="P23" s="116"/>
-      <c r="Q23" s="116"/>
-      <c r="R23" s="99"/>
-      <c r="S23" s="99"/>
-      <c r="T23" s="99"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="82"/>
+      <c r="S23" s="82"/>
+      <c r="T23" s="82"/>
     </row>
     <row r="24" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
@@ -2769,14 +2782,14 @@
       <c r="I24" s="26"/>
       <c r="J24" s="26"/>
       <c r="K24" s="58"/>
-      <c r="M24" s="81"/>
-      <c r="N24" s="81"/>
-      <c r="O24" s="81"/>
-      <c r="P24" s="81"/>
-      <c r="Q24" s="81"/>
-      <c r="R24" s="81"/>
-      <c r="S24" s="81"/>
-      <c r="T24" s="81"/>
+      <c r="M24" s="124"/>
+      <c r="N24" s="124"/>
+      <c r="O24" s="124"/>
+      <c r="P24" s="124"/>
+      <c r="Q24" s="124"/>
+      <c r="R24" s="124"/>
+      <c r="S24" s="124"/>
+      <c r="T24" s="124"/>
     </row>
     <row r="25" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="57"/>
@@ -2788,14 +2801,14 @@
       <c r="I25" s="26"/>
       <c r="J25" s="26"/>
       <c r="K25" s="58"/>
-      <c r="M25" s="79"/>
-      <c r="N25" s="79"/>
-      <c r="O25" s="79"/>
-      <c r="P25" s="79"/>
-      <c r="Q25" s="79"/>
-      <c r="R25" s="79"/>
-      <c r="S25" s="79"/>
-      <c r="T25" s="79"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="78"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="78"/>
     </row>
     <row r="26" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="61"/>
@@ -2807,14 +2820,14 @@
       <c r="I26" s="26"/>
       <c r="J26" s="26"/>
       <c r="K26" s="58"/>
-      <c r="M26" s="79"/>
-      <c r="N26" s="79"/>
-      <c r="O26" s="79"/>
-      <c r="P26" s="79"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="79"/>
-      <c r="S26" s="79"/>
-      <c r="T26" s="79"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="78"/>
+      <c r="O26" s="78"/>
+      <c r="P26" s="78"/>
+      <c r="Q26" s="78"/>
+      <c r="R26" s="78"/>
+      <c r="S26" s="78"/>
+      <c r="T26" s="78"/>
     </row>
     <row r="27" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="61"/>
@@ -2826,14 +2839,14 @@
       <c r="I27" s="26"/>
       <c r="J27" s="26"/>
       <c r="K27" s="58"/>
-      <c r="M27" s="79"/>
-      <c r="N27" s="79"/>
-      <c r="O27" s="79"/>
-      <c r="P27" s="79"/>
-      <c r="Q27" s="79"/>
-      <c r="R27" s="79"/>
-      <c r="S27" s="79"/>
-      <c r="T27" s="79"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="78"/>
+      <c r="O27" s="78"/>
+      <c r="P27" s="78"/>
+      <c r="Q27" s="78"/>
+      <c r="R27" s="78"/>
+      <c r="S27" s="78"/>
+      <c r="T27" s="78"/>
     </row>
     <row r="28" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="57"/>
@@ -2845,14 +2858,14 @@
       <c r="I28" s="63"/>
       <c r="J28" s="20"/>
       <c r="K28" s="60"/>
-      <c r="M28" s="124"/>
-      <c r="N28" s="79"/>
-      <c r="O28" s="79"/>
-      <c r="P28" s="79"/>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="79"/>
-      <c r="S28" s="79"/>
-      <c r="T28" s="79"/>
+      <c r="M28" s="77"/>
+      <c r="N28" s="78"/>
+      <c r="O28" s="78"/>
+      <c r="P28" s="78"/>
+      <c r="Q28" s="78"/>
+      <c r="R28" s="78"/>
+      <c r="S28" s="78"/>
+      <c r="T28" s="78"/>
     </row>
     <row r="29" spans="2:20" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="57"/>
@@ -2922,29 +2935,18 @@
       <c r="D34" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="M12:T12"/>
-    <mergeCell ref="N10:U10"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
+  <mergeCells count="34">
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="M12:T13"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="M24:T24"/>
+    <mergeCell ref="M25:T25"/>
+    <mergeCell ref="M26:T26"/>
+    <mergeCell ref="R18:S18"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="M28:T28"/>
-    <mergeCell ref="N2:O2"/>
     <mergeCell ref="S17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="M13:T13"/>
     <mergeCell ref="M14:T14"/>
     <mergeCell ref="R15:T15"/>
     <mergeCell ref="M16:T16"/>
@@ -2954,10 +2956,20 @@
     <mergeCell ref="M27:T27"/>
     <mergeCell ref="R22:T22"/>
     <mergeCell ref="M23:Q23"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="M24:T24"/>
-    <mergeCell ref="M25:T25"/>
-    <mergeCell ref="M26:T26"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="N10:U10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0" right="0.28000000000000003" top="0.22" bottom="0.196850393700787" header="0.28000000000000003" footer="0.196850393700787"/>

</xml_diff>